<commit_message>
20210727 02 update from local
</commit_message>
<xml_diff>
--- a/data/VC_ARC_F2_Crosses organised_counted_measured_new.xlsx
+++ b/data/VC_ARC_F2_Crosses organised_counted_measured_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brettell/Documents/Repositories/medaka_vertebrae/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CC6D981-D267-2441-9070-3B5C1A18793F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523688DC-7E91-584C-8D5E-64DFC98AD468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="13920" tabRatio="878" activeTab="1" xr2:uid="{060F9272-4C6F-4A03-BD1D-30667ED1EBF0}"/>
+    <workbookView xWindow="-34160" yWindow="1080" windowWidth="28800" windowHeight="13920" tabRatio="878" activeTab="1" xr2:uid="{060F9272-4C6F-4A03-BD1D-30667ED1EBF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Details of crosses" sheetId="20" r:id="rId1"/>
@@ -30429,7 +30429,7 @@
   <dimension ref="A1:N131"/>
   <sheetViews>
     <sheetView zoomScale="65" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33386,7 +33386,7 @@
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33546,23 +33546,23 @@
         <v>21.001000000000001</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L22" si="2">H3/I3</f>
+        <f t="shared" ref="L3:L11" si="2">H3/I3</f>
         <v>0.67519353752945133</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M22" si="3">H3/J3</f>
+        <f t="shared" ref="M3:M11" si="3">H3/J3</f>
         <v>0.40305404862366884</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N22" si="4">I3/J3</f>
+        <f t="shared" ref="N3:N11" si="4">I3/J3</f>
         <v>0.59694595137633111</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O22" si="5">H3/K3</f>
+        <f t="shared" ref="O3:O11" si="5">H3/K3</f>
         <v>0.28655778296271606</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P22" si="6">I3/K3</f>
+        <f t="shared" ref="P3:P11" si="6">I3/K3</f>
         <v>0.42440836150659489</v>
       </c>
     </row>
@@ -33660,20 +33660,20 @@
         <v>18.550999999999998</v>
       </c>
       <c r="L5">
-        <f>I4/I5</f>
-        <v>1.2016612200435728</v>
+        <f t="shared" si="2"/>
+        <v>0.75721677559912848</v>
       </c>
       <c r="M5">
-        <f>I4/J5</f>
-        <v>0.68384347152266556</v>
+        <f t="shared" si="3"/>
+        <v>0.43091824874079809</v>
       </c>
       <c r="N5">
         <f t="shared" si="4"/>
         <v>0.5690817512592018</v>
       </c>
       <c r="O5">
-        <f>I4/K5</f>
-        <v>0.475715594846639</v>
+        <f t="shared" si="5"/>
+        <v>0.29976820656568381</v>
       </c>
       <c r="P5">
         <f t="shared" si="6"/>
@@ -33717,20 +33717,20 @@
         <v>20.291</v>
       </c>
       <c r="L6">
-        <f>K4/I6</f>
-        <v>2.4669019226089071</v>
+        <f t="shared" si="2"/>
+        <v>0.75444146994402539</v>
       </c>
       <c r="M6">
-        <f>K4/J6</f>
-        <v>1.4060896102094604</v>
+        <f t="shared" si="3"/>
+        <v>0.4300180330142877</v>
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
         <v>0.56998196698571235</v>
       </c>
       <c r="O6">
-        <f>K4/K6</f>
-        <v>0.99911290720023649</v>
+        <f t="shared" si="5"/>
+        <v>0.30555418658518557</v>
       </c>
       <c r="P6">
         <f t="shared" si="6"/>
@@ -34059,23 +34059,23 @@
         <v>19.475999999999999</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="L3:L22" si="7">H14/I14</f>
         <v>0.76876136068553624</v>
       </c>
       <c r="M14">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="M3:M22" si="8">H14/J14</f>
         <v>0.43463260662115538</v>
       </c>
       <c r="N14">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="N3:N22" si="9">I14/J14</f>
         <v>0.56536739337884456</v>
       </c>
       <c r="O14">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="O3:O22" si="10">H14/K14</f>
         <v>0.30401519819264738</v>
       </c>
       <c r="P14">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="P3:P22" si="11">I14/K14</f>
         <v>0.39546108030396387</v>
       </c>
     </row>
@@ -34116,23 +34116,23 @@
         <v>19.853999999999999</v>
       </c>
       <c r="L15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.65690824705462325</v>
       </c>
       <c r="M15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.39646627881921997</v>
       </c>
       <c r="N15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.60353372118078008</v>
       </c>
       <c r="O15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.27802961619824718</v>
       </c>
       <c r="P15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.42323964944091874</v>
       </c>
     </row>
@@ -34173,23 +34173,23 @@
         <v>20.706</v>
       </c>
       <c r="L16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.74162110767768008</v>
       </c>
       <c r="M16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.4258223010782039</v>
       </c>
       <c r="N16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.57417769892179604</v>
       </c>
       <c r="O16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.30136192407997686</v>
       </c>
       <c r="P16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.40635564570655847</v>
       </c>
     </row>
@@ -34230,23 +34230,23 @@
         <v>21.602</v>
       </c>
       <c r="L17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.77243367935409457</v>
       </c>
       <c r="M17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.43580399557493327</v>
       </c>
       <c r="N17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.56419600442506668</v>
       </c>
       <c r="O17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.31001759096379966</v>
       </c>
       <c r="P17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.40135172669197294</v>
       </c>
     </row>
@@ -34287,23 +34287,23 @@
         <v>22.756</v>
       </c>
       <c r="L18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.68132667914327305</v>
       </c>
       <c r="M18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.40523158740956033</v>
       </c>
       <c r="N18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.59476841259043967</v>
       </c>
       <c r="O18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.28796800843733522</v>
       </c>
       <c r="P18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.4226577605906135</v>
       </c>
     </row>
@@ -34344,23 +34344,23 @@
         <v>21.917000000000002</v>
       </c>
       <c r="L19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.78535271943995688</v>
       </c>
       <c r="M19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.43988658985341139</v>
       </c>
       <c r="N19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.56011341014658866</v>
       </c>
       <c r="O19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33270976867271979</v>
       </c>
       <c r="P19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.42364374686316558</v>
       </c>
     </row>
@@ -34401,23 +34401,23 @@
         <v>23.056999999999999</v>
       </c>
       <c r="L22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.65746232377248415</v>
       </c>
       <c r="M22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.39666803543145418</v>
       </c>
       <c r="N22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.60333196456854576</v>
       </c>
       <c r="O22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.29327319252287809</v>
       </c>
       <c r="P22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.44606843908574406</v>
       </c>
     </row>
@@ -34458,23 +34458,23 @@
         <v>24.373000000000001</v>
       </c>
       <c r="L23">
-        <f t="shared" ref="L23:L31" si="7">H23/I23</f>
+        <f t="shared" ref="L23:L31" si="12">H23/I23</f>
         <v>0.71017764255569726</v>
       </c>
       <c r="M23">
-        <f t="shared" ref="M23:M31" si="8">H23/J23</f>
+        <f t="shared" ref="M23:M31" si="13">H23/J23</f>
         <v>0.41526542324246768</v>
       </c>
       <c r="N23">
-        <f t="shared" ref="N23:N31" si="9">I23/J23</f>
+        <f t="shared" ref="N23:N31" si="14">I23/J23</f>
         <v>0.58473457675753227</v>
       </c>
       <c r="O23">
-        <f t="shared" ref="O23:O31" si="10">H23/K23</f>
+        <f t="shared" ref="O23:O31" si="15">H23/K23</f>
         <v>0.29688589833011936</v>
       </c>
       <c r="P23">
-        <f t="shared" ref="P23:P31" si="11">I23/K23</f>
+        <f t="shared" ref="P23:P31" si="16">I23/K23</f>
         <v>0.41804455750215402</v>
       </c>
     </row>
@@ -34515,23 +34515,23 @@
         <v>25.573</v>
       </c>
       <c r="L24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.69746524938675392</v>
       </c>
       <c r="M24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.41088631984585744</v>
       </c>
       <c r="N24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.58911368015414267</v>
       </c>
       <c r="O24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30019942908536346</v>
       </c>
       <c r="P24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.43041489070504046</v>
       </c>
     </row>
@@ -34572,23 +34572,23 @@
         <v>23.056000000000001</v>
       </c>
       <c r="L25">
-        <f t="shared" ref="L25" si="12">H25/I25</f>
+        <f t="shared" ref="L25" si="17">H25/I25</f>
         <v>0.82763824512234563</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25" si="13">H25/J25</f>
+        <f t="shared" ref="M25" si="18">H25/J25</f>
         <v>0.45284576820996758</v>
       </c>
       <c r="N25">
-        <f t="shared" ref="N25" si="14">I25/J25</f>
+        <f t="shared" ref="N25" si="19">I25/J25</f>
         <v>0.54715423179003242</v>
       </c>
       <c r="O25">
-        <f t="shared" ref="O25" si="15">H25/K25</f>
+        <f t="shared" ref="O25" si="20">H25/K25</f>
         <v>0.3330152671755725</v>
       </c>
       <c r="P25">
-        <f t="shared" ref="P25" si="16">I25/K25</f>
+        <f t="shared" ref="P25" si="21">I25/K25</f>
         <v>0.40236814712005547</v>
       </c>
     </row>
@@ -34629,23 +34629,23 @@
         <v>23.341999999999999</v>
       </c>
       <c r="L26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.64568010199078163</v>
       </c>
       <c r="M26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.39234848936297001</v>
       </c>
       <c r="N26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.60765151063702993</v>
       </c>
       <c r="O26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.28206666095450261</v>
       </c>
       <c r="P26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.43685202639019793</v>
       </c>
     </row>
@@ -34686,23 +34686,23 @@
         <v>24.568000000000001</v>
       </c>
       <c r="L27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.67061850932818667</v>
       </c>
       <c r="M27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.40141929805259102</v>
       </c>
       <c r="N27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.59858070194740898</v>
       </c>
       <c r="O27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.29701237381960272</v>
       </c>
       <c r="P27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.44289319439921848</v>
       </c>
     </row>
@@ -34743,23 +34743,23 @@
         <v>23.326000000000001</v>
       </c>
       <c r="L28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.79545454545454553</v>
       </c>
       <c r="M28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.44303797468354433</v>
       </c>
       <c r="N28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.55696202531645578</v>
       </c>
       <c r="O28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.31960044585441139</v>
       </c>
       <c r="P28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.4017834176455457</v>
       </c>
     </row>
@@ -34800,23 +34800,23 @@
         <v>23.63</v>
       </c>
       <c r="L29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.68682795698924726</v>
       </c>
       <c r="M29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.40717131474103579</v>
       </c>
       <c r="N29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.59282868525896415</v>
       </c>
       <c r="O29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.28112568768514601</v>
       </c>
       <c r="P29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.40931019889970383</v>
       </c>
     </row>
@@ -34857,23 +34857,23 @@
         <v>22.731999999999999</v>
       </c>
       <c r="L30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.63751748950629616</v>
       </c>
       <c r="M30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.3893194995422643</v>
       </c>
       <c r="N30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.61068050045773581</v>
       </c>
       <c r="O30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.28061763153264119</v>
       </c>
       <c r="P30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.44017244413162065</v>
       </c>
     </row>
@@ -34914,23 +34914,23 @@
         <v>24.262</v>
       </c>
       <c r="L31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.69611105828658359</v>
       </c>
       <c r="M31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.41041596591546131</v>
       </c>
       <c r="N31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.58958403408453852</v>
       </c>
       <c r="O31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.30174758882202618</v>
       </c>
       <c r="P31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.4334762179540021</v>
       </c>
     </row>
@@ -37773,7 +37773,7 @@
   </sheetPr>
   <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -44102,7 +44102,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>